<commit_message>
HW-75 BMS AFE Rev 4.1 - Tented all vias - Added pcb prints to the pdf - Updated all project outputs
</commit_message>
<xml_diff>
--- a/MSXII_BMS_AFE/Project Outputs for BMS_AFE/BMS_AFE_4.1.xlsx
+++ b/MSXII_BMS_AFE/Project Outputs for BMS_AFE/BMS_AFE_4.1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDA56C48-411E-422A-BFBB-B9CA49E532BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9CCE051-5BDF-43A6-A51B-4DE1DE47FC5D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30" yWindow="75" windowWidth="15165" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="192">
   <si>
     <t>Title</t>
   </si>
@@ -104,7 +104,7 @@
     <t>Taiping Li</t>
   </si>
   <si>
-    <t>2018-12-22 9:44:29 PM</t>
+    <t>2018-12-22 10:02:02 PM</t>
   </si>
   <si>
     <t>1</t>
@@ -113,7 +113,7 @@
     <t>CAD</t>
   </si>
   <si>
-    <t>165</t>
+    <t>173</t>
   </si>
   <si>
     <t>LibRef</t>
@@ -152,6 +152,9 @@
     <t>CONN 10POS MICRO-FIT 3mm</t>
   </si>
   <si>
+    <t>CONN 5POS HEADR MALE 0.1in</t>
+  </si>
+  <si>
     <t>CONN 12POS MICRO-FIT 3mm</t>
   </si>
   <si>
@@ -218,7 +221,7 @@
     <t>C1, C2</t>
   </si>
   <si>
-    <t>C3, C4, C5, C39</t>
+    <t>C3, C4, C5, C6, C39</t>
   </si>
   <si>
     <t>C7, C8, C9, C10, C11, C12, C13, C14, C15, C16, C17, C18, C19, C20, C21, C22, C23, C24, C25, C26, C27, C28, C29, C30, C31, C32, C33, C34, C35, C36, C37, C38, C42</t>
@@ -248,6 +251,9 @@
     <t>P4</t>
   </si>
   <si>
+    <t>P5</t>
+  </si>
+  <si>
     <t>P6</t>
   </si>
   <si>
@@ -266,10 +272,10 @@
     <t>R1, R2, R53, R54, R55, R56, R57, R58, R59, R60, R61, R62, R63, R64, R65, R75</t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R5, R6, R7, R8</t>
+    <t>R3, R4, R11, R12, R52, R66</t>
+  </si>
+  <si>
+    <t>R5, R6, R7, R8, R10</t>
   </si>
   <si>
     <t>R9</t>
@@ -401,13 +407,16 @@
     <t>43045-1027</t>
   </si>
   <si>
+    <t>0022284050</t>
+  </si>
+  <si>
     <t>0430451227</t>
   </si>
   <si>
-    <t>0430450227</t>
-  </si>
-  <si>
-    <t>43045-1427</t>
+    <t>43045-0227</t>
+  </si>
+  <si>
+    <t>0430451427</t>
   </si>
   <si>
     <t>NSV1C201MZ4T1G</t>
@@ -503,6 +512,9 @@
     <t>WM7488-ND</t>
   </si>
   <si>
+    <t>WM50014-05-ND</t>
+  </si>
+  <si>
     <t>WM10697-ND</t>
   </si>
   <si>
@@ -575,10 +587,10 @@
     <t>C:\Users\Taiping\Documents\MidnightSun\hardware\MSXII_BMS_AFE\BMS_AFE.PrjPcb</t>
   </si>
   <si>
-    <t>01 - Standard</t>
-  </si>
-  <si>
-    <t>9:44:29 PM</t>
+    <t>None</t>
+  </si>
+  <si>
+    <t>10:02:02 PM</t>
   </si>
   <si>
     <t>2018-12-22</t>
@@ -1174,7 +1186,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:J45"/>
+  <dimension ref="A2:J46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
@@ -1280,28 +1292,28 @@
         <v>30</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="I11" s="28" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1309,19 +1321,19 @@
         <v>31</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="G12" s="3">
         <v>0.57999999999999996</v>
@@ -1338,28 +1350,28 @@
         <v>32</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="G13" s="3">
         <v>0.39</v>
       </c>
       <c r="H13" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I13" s="8">
-        <v>1.58</v>
+        <v>1.97</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1367,19 +1379,19 @@
         <v>33</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F14" s="33" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="G14" s="3">
         <v>0.28000000000000003</v>
@@ -1396,19 +1408,19 @@
         <v>34</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F15" s="33" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G15" s="3">
         <v>0.23</v>
@@ -1425,19 +1437,19 @@
         <v>35</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G16" s="3">
         <v>0.28000000000000003</v>
@@ -1454,19 +1466,19 @@
         <v>36</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F17" s="33" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="G17" s="3">
         <v>1.07</v>
@@ -1483,19 +1495,19 @@
         <v>37</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="G18" s="3">
         <v>0.19</v>
@@ -1512,19 +1524,19 @@
         <v>38</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="G19" s="3">
         <v>0.19</v>
@@ -1541,19 +1553,19 @@
         <v>39</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G20" s="3">
         <v>2.61</v>
@@ -1570,19 +1582,19 @@
         <v>40</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G21" s="3">
         <v>1.06</v>
@@ -1599,19 +1611,19 @@
         <v>41</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="G22" s="3">
         <v>3.06</v>
@@ -1628,42 +1640,48 @@
         <v>42</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F23" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="8"/>
+        <v>162</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1</v>
+      </c>
+      <c r="I23" s="8">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="24" spans="1:9" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="29" t="s">
         <v>43</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F24" s="33" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1674,28 +1692,28 @@
         <v>44</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F25" s="33" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G25" s="3">
-        <v>4.43</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="H25" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I25" s="8">
-        <v>4.43</v>
+        <v>2.29</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1703,57 +1721,51 @@
         <v>45</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F26" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="G26" s="3">
-        <v>0.94</v>
-      </c>
-      <c r="H26" s="3">
-        <v>1</v>
-      </c>
-      <c r="I26" s="8">
-        <v>0.94</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="8"/>
     </row>
     <row r="27" spans="1:9" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D27" s="32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F27" s="33" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="G27" s="3">
-        <v>0.42</v>
+        <v>0.94</v>
       </c>
       <c r="H27" s="3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I27" s="8">
-        <v>5.04</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1761,28 +1773,28 @@
         <v>47</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F28" s="33" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="G28" s="3">
-        <v>0.03</v>
+        <v>0.42</v>
       </c>
       <c r="H28" s="3">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I28" s="8">
-        <v>0.52</v>
+        <v>5.04</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1790,28 +1802,28 @@
         <v>48</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F29" s="33" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="G29" s="3">
-        <v>0.23</v>
+        <v>0.03</v>
       </c>
       <c r="H29" s="3">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I29" s="8">
-        <v>0.23</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1819,28 +1831,28 @@
         <v>49</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F30" s="33" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="G30" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.23</v>
       </c>
       <c r="H30" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I30" s="8">
-        <v>0.54</v>
+        <v>1.39</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1848,28 +1860,28 @@
         <v>50</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F31" s="33" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G31" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="H31" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I31" s="8">
-        <v>0.14000000000000001</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1877,19 +1889,19 @@
         <v>51</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F32" s="33" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="G32" s="3">
         <v>0.14000000000000001</v>
@@ -1906,28 +1918,28 @@
         <v>52</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F33" s="33" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G33" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="H33" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33" s="8">
-        <v>0.27</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1935,28 +1947,28 @@
         <v>53</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F34" s="33" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G34" s="3">
-        <v>0.2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H34" s="3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I34" s="8">
-        <v>2.35</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1964,28 +1976,28 @@
         <v>54</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F35" s="33" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="G35" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="H35" s="3">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="I35" s="8">
-        <v>13.19</v>
+        <v>2.35</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1993,28 +2005,28 @@
         <v>55</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F36" s="33" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="G36" s="3">
-        <v>0.48</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H36" s="3">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="I36" s="8">
-        <v>1.9</v>
+        <v>13.19</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2022,28 +2034,28 @@
         <v>56</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C37" s="31" t="s">
         <v>109</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F37" s="33" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="G37" s="3">
-        <v>1.0900000000000001</v>
+        <v>0.48</v>
       </c>
       <c r="H37" s="3">
         <v>4</v>
       </c>
       <c r="I37" s="8">
-        <v>4.3499999999999996</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2051,28 +2063,28 @@
         <v>57</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F38" s="33" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="G38" s="3">
-        <v>0.95</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="H38" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I38" s="8">
-        <v>0.95</v>
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2080,28 +2092,28 @@
         <v>58</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D39" s="32" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F39" s="33" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G39" s="3">
-        <v>25.94</v>
+        <v>0.95</v>
       </c>
       <c r="H39" s="3">
         <v>1</v>
       </c>
       <c r="I39" s="8">
-        <v>25.94</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2109,28 +2121,28 @@
         <v>59</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D40" s="32" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F40" s="33" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="G40" s="3">
-        <v>1.2</v>
+        <v>25.94</v>
       </c>
       <c r="H40" s="3">
         <v>1</v>
       </c>
       <c r="I40" s="8">
-        <v>1.2</v>
+        <v>25.94</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2138,28 +2150,28 @@
         <v>60</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F41" s="33" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G41" s="3">
-        <v>1.1599999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="H41" s="3">
         <v>1</v>
       </c>
       <c r="I41" s="8">
-        <v>1.1599999999999999</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2167,60 +2179,77 @@
         <v>61</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E42" s="29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F42" s="33" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="G42" s="3">
-        <v>2.52</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="H42" s="3">
         <v>1</v>
       </c>
       <c r="I42" s="8">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="F43" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="G43" s="3">
         <v>2.52</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="9"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="3" t="s">
+      <c r="H43" s="3">
+        <v>1</v>
+      </c>
+      <c r="I43" s="8">
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" s="9"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I43" s="12">
-        <f>SUM(I12:I42)</f>
-        <v>105.74</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="13"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="15"/>
+      <c r="I44" s="12">
+        <f>SUM(I12:I43)</f>
+        <v>105.62</v>
+      </c>
     </row>
     <row r="45" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="14"/>
+      <c r="A45" s="13"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
       <c r="D45" s="13"/>
@@ -2231,112 +2260,127 @@
       <c r="I45" s="13"/>
       <c r="J45" s="15"/>
     </row>
+    <row r="46" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="15"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1" tooltip="Component" display="'Murata" xr:uid="{424D8D39-C19A-4FEC-8A35-6253C00E713F}"/>
-    <hyperlink ref="C13" r:id="rId2" tooltip="Component" display="'Taiyo Yuden" xr:uid="{0B97BA1B-2960-452B-8206-EC0F85D22F90}"/>
-    <hyperlink ref="C14" r:id="rId3" tooltip="Component" display="'KEMET" xr:uid="{73C718DC-A8A9-4947-A2DA-07A72D734E0E}"/>
-    <hyperlink ref="C15" r:id="rId4" tooltip="Component" display="'Kyocera AVX" xr:uid="{C773F878-AF00-4C6C-B093-73F4AB170460}"/>
-    <hyperlink ref="C16" r:id="rId5" tooltip="Component" display="'Diodes" xr:uid="{E59CD8B7-6EBA-4232-A028-736ECE5065FD}"/>
-    <hyperlink ref="C17" r:id="rId6" tooltip="Component" display="'Littelfuse" xr:uid="{0D22ACBF-2AA7-476B-8236-22928F0A47AA}"/>
-    <hyperlink ref="C18" r:id="rId7" tooltip="Component" display="'Wurth Electronics" xr:uid="{DCF26399-D62F-45B4-AB1A-116ADC3B6FE7}"/>
-    <hyperlink ref="C19" r:id="rId8" tooltip="Component" display="'Wurth Electronics" xr:uid="{08616433-CF0B-48E4-A904-365E4813B60B}"/>
-    <hyperlink ref="C20" r:id="rId9" tooltip="Component" display="'Molex" xr:uid="{00412847-6BA9-4651-8310-15252E42B83F}"/>
-    <hyperlink ref="C21" r:id="rId10" tooltip="Component" display="'Molex" xr:uid="{C287978C-3121-4AA3-B927-A26B40BF70FE}"/>
-    <hyperlink ref="C22" r:id="rId11" tooltip="Component" display="'Molex" xr:uid="{E3956F3D-6147-4A6C-A364-558146DDE801}"/>
-    <hyperlink ref="C23" r:id="rId12" tooltip="Component" display="'Molex" xr:uid="{94F3F015-EE26-49BF-9381-7058C016B8EC}"/>
-    <hyperlink ref="C24" r:id="rId13" tooltip="Component" display="'Molex" xr:uid="{6CE6B665-00FC-4D12-AD97-5252636B1679}"/>
-    <hyperlink ref="C25" r:id="rId14" tooltip="Component" display="'Molex" xr:uid="{46986AE6-C24E-4A3C-958A-C944934F239A}"/>
-    <hyperlink ref="C26" r:id="rId15" tooltip="Component" display="'ON Semiconductor" xr:uid="{AE410FE4-8299-4991-8FC6-045B9F0C6B01}"/>
-    <hyperlink ref="C27" r:id="rId16" tooltip="Component" display="'Diodes" xr:uid="{9E968524-93DF-4A26-8BDE-0BCB391AD804}"/>
-    <hyperlink ref="C28" r:id="rId17" tooltip="Component" display="'Yageo" xr:uid="{98B63C66-17F7-47BD-9F28-2FEDBC849480}"/>
-    <hyperlink ref="C29" r:id="rId18" tooltip="Component" display="'Vishay Dale" xr:uid="{791ED5D0-6277-42BA-BCD3-890BBF0F1C3F}"/>
-    <hyperlink ref="C30" r:id="rId19" tooltip="Component" display="'Yageo Phycomp" xr:uid="{71533B63-7A43-4627-ABC5-44468FC6FB40}"/>
-    <hyperlink ref="C31" r:id="rId20" tooltip="Component" display="'Yageo" xr:uid="{D9BA2338-F1B6-4EC5-BE9A-8BD9D2C0DD8B}"/>
-    <hyperlink ref="C32" r:id="rId21" tooltip="Component" display="'Yageo" xr:uid="{1E0E23FB-FEB9-4121-94E1-2D0A7747D23A}"/>
-    <hyperlink ref="C33" r:id="rId22" tooltip="Component" display="'Yageo" xr:uid="{F78EBC05-51A1-4EF1-9B65-E78AC917A48E}"/>
-    <hyperlink ref="C34" r:id="rId23" tooltip="Component" display="'Panasonic" xr:uid="{A9317D52-9696-4A46-A521-CCFB2363CA61}"/>
-    <hyperlink ref="C35" r:id="rId24" tooltip="Component" display="'Stackpole Electronics" xr:uid="{9DC50234-2B29-4F3B-9B62-D61BF215C738}"/>
-    <hyperlink ref="C36" r:id="rId25" tooltip="Component" display="'Panasonic" xr:uid="{5079A352-5457-41D4-93C7-B06B6465A634}"/>
-    <hyperlink ref="C37" r:id="rId26" tooltip="Component" display="'Vishay Beyschlag" xr:uid="{E6979880-6479-4758-8405-B5FA98B426CC}"/>
-    <hyperlink ref="C38" r:id="rId27" tooltip="Component" display="'Murata" xr:uid="{89E6A000-D722-46AF-80B0-98124B54206F}"/>
-    <hyperlink ref="C39" r:id="rId28" tooltip="Component" display="'Analog Devices / Linear Technology" xr:uid="{C6CF9CE3-C070-499C-A8C0-6CA3F2E0D2F3}"/>
-    <hyperlink ref="C40" r:id="rId29" tooltip="Component" display="'Texas Instruments" xr:uid="{791ECD81-2298-4382-90ED-3AE82C3E80F1}"/>
-    <hyperlink ref="C41" r:id="rId30" tooltip="Component" display="'Texas Instruments" xr:uid="{4D85487F-31A5-4D8C-9F2B-31E79A9D32F2}"/>
-    <hyperlink ref="C42" r:id="rId31" tooltip="Component" display="'Bourns" xr:uid="{DAFB5CEA-A413-4DAF-A90C-75DF1CFF5306}"/>
-    <hyperlink ref="D12" r:id="rId32" tooltip="Manufacturer" display="'GCM21BR72A104KA37L" xr:uid="{70870A30-BAEE-406A-94A9-66B80FA49C64}"/>
-    <hyperlink ref="D13" r:id="rId33" tooltip="Manufacturer" display="'UMK107AB7105KA-T" xr:uid="{2CD371DF-00BE-49F6-BA62-6B1B107D583E}"/>
-    <hyperlink ref="D14" r:id="rId34" tooltip="Manufacturer" display="'C0603C103J5JAC7867" xr:uid="{C19F6165-CEEC-48A1-AA57-3893E76BBD14}"/>
-    <hyperlink ref="D15" r:id="rId35" tooltip="Manufacturer" display="'06035C-104KAT2A" xr:uid="{E8FF6E0E-214C-4645-9574-7D2E17835474}"/>
-    <hyperlink ref="D16" r:id="rId36" tooltip="Manufacturer" display="'MMSZ5235B-7-F" xr:uid="{1AD7B45E-9E30-40D9-AAD5-35FEB76224C9}"/>
-    <hyperlink ref="D17" r:id="rId37" tooltip="Manufacturer" display="'0466.375NR" xr:uid="{65AD346B-C8C8-4AD4-AD89-9485BA131A17}"/>
-    <hyperlink ref="D18" r:id="rId38" tooltip="Manufacturer" display="'150060RS75000" xr:uid="{290D53F8-2BC4-4564-9886-E3B0AA76ED7F}"/>
-    <hyperlink ref="D19" r:id="rId39" tooltip="Manufacturer" display="'150060VS75000" xr:uid="{0CE91E9E-E1EA-4450-9A5B-7529BF3D0334}"/>
-    <hyperlink ref="D20" r:id="rId40" tooltip="Manufacturer" display="'43045-0827" xr:uid="{CD427EBF-CFEC-4E13-8A63-FE5D52AAA1B8}"/>
-    <hyperlink ref="D21" r:id="rId41" tooltip="Manufacturer" display="'560020-0220" xr:uid="{464036C1-FBD1-45C9-98CE-C605CE77F058}"/>
-    <hyperlink ref="D22" r:id="rId42" tooltip="Manufacturer" display="'43045-1027" xr:uid="{DA1DB2CE-1591-4F53-BCD4-3AC716CA690E}"/>
-    <hyperlink ref="D23" r:id="rId43" tooltip="Manufacturer" display="'0430451227" xr:uid="{4B224634-740B-4C42-8BB1-FFE3F0B2E1E9}"/>
-    <hyperlink ref="D24" r:id="rId44" tooltip="Manufacturer" display="'0430450227" xr:uid="{654479DC-1ED5-474E-9234-2B39CD6C7215}"/>
-    <hyperlink ref="D25" r:id="rId45" tooltip="Manufacturer" display="'43045-1427" xr:uid="{DA6A2729-4BC4-459A-A6BF-912A9B58BD5A}"/>
-    <hyperlink ref="D26" r:id="rId46" tooltip="Manufacturer" display="'NSV1C201MZ4T1G" xr:uid="{E64FFCA4-5A92-43D3-AFBA-6BCF1A9CB59D}"/>
-    <hyperlink ref="D27" r:id="rId47" tooltip="Manufacturer" display="'DMP3099L-7" xr:uid="{7BA53FF4-E099-4B5F-98B1-AB9117FE5AE6}"/>
-    <hyperlink ref="D28" r:id="rId48" tooltip="Manufacturer" display="'RC0603FR-07100RL" xr:uid="{95221AB5-F19F-4823-A9C0-F7E676848F11}"/>
-    <hyperlink ref="D29" r:id="rId49" tooltip="Manufacturer" display="'CRCW06030000Z0EAHP" xr:uid="{AE406DBD-3D28-4694-9CC2-D30686A9DCAC}"/>
-    <hyperlink ref="D30" r:id="rId50" tooltip="Manufacturer" display="'RC0603FR-074K7L" xr:uid="{B2F98D80-C8AF-4C95-BABA-9A30CD4ED9FF}"/>
-    <hyperlink ref="D31" r:id="rId51" tooltip="Manufacturer" display="'RC0603FR-071K4L" xr:uid="{892F2EEF-51C7-4371-8912-E7F196C8D3B5}"/>
-    <hyperlink ref="D32" r:id="rId52" tooltip="Manufacturer" display="'RC0603FR-07604RL" xr:uid="{FA0F7853-2F12-4173-817D-ECBF4E4D8A27}"/>
-    <hyperlink ref="D33" r:id="rId53" tooltip="Manufacturer" display="'RC0603JR-07100KL" xr:uid="{2D924FDC-E6FE-4001-BCE2-7EA69577455C}"/>
-    <hyperlink ref="D34" r:id="rId54" tooltip="Manufacturer" display="'ERJPA3F3301V" xr:uid="{245D7825-EFF5-46A6-ABEB-D7391C32EA11}"/>
-    <hyperlink ref="D35" r:id="rId55" tooltip="Manufacturer" display="'RPC2512JT33R0" xr:uid="{716C65CD-BFE7-4376-8431-9B4191FCACA8}"/>
-    <hyperlink ref="D36" r:id="rId56" tooltip="Manufacturer" display="'ERA-3AEB620V" xr:uid="{EF9EE980-A79B-40AB-992E-998BDD4CD589}"/>
-    <hyperlink ref="D37" r:id="rId57" tooltip="Manufacturer" display="'ACASA1002S1002P100" xr:uid="{F883FF3F-14F1-4F5C-AE30-6B4111CAD6EF}"/>
-    <hyperlink ref="D38" r:id="rId58" tooltip="Manufacturer" display="'NXRT15XH103FA1B030" xr:uid="{38A4C4E5-5F13-4FDB-AF9E-A75BBDF35DAA}"/>
-    <hyperlink ref="D39" r:id="rId59" tooltip="Manufacturer" display="'LTC6804IG-1#PBF" xr:uid="{25F736A0-F2CD-4253-8F9D-437F9FDE2E41}"/>
-    <hyperlink ref="D40" r:id="rId60" tooltip="Manufacturer" display="'CD74HC4067SM96" xr:uid="{EE5AE4F2-6872-4116-A180-EB87ECBF36EB}"/>
-    <hyperlink ref="D41" r:id="rId61" tooltip="Manufacturer" display="'TLV316QDBVRQ1" xr:uid="{2F3B3C22-FBDB-4947-9666-78623FBAB705}"/>
-    <hyperlink ref="D42" r:id="rId62" tooltip="Manufacturer" display="'PT61018AAPEL-S" xr:uid="{977035A6-1075-4B3B-BB0F-51973851B61C}"/>
-    <hyperlink ref="F12" r:id="rId63" tooltip="Supplier" display="'490-4789-1-ND" xr:uid="{DD48C287-CEBD-44E5-8A8F-D13E57D590F4}"/>
-    <hyperlink ref="F13" r:id="rId64" tooltip="Supplier" display="'587-3247-1-ND" xr:uid="{6A43137E-B5C2-45DD-8600-B44BFFF93392}"/>
-    <hyperlink ref="F14" r:id="rId65" tooltip="Supplier" display="'399-13384-1-ND" xr:uid="{8BE0BA62-87B5-4B59-9416-6FA8EFBF6F7E}"/>
-    <hyperlink ref="F15" r:id="rId66" tooltip="Supplier" display="'478-5052-1-ND" xr:uid="{615FAC08-F77F-45C3-B212-6C495E706DB3}"/>
-    <hyperlink ref="F16" r:id="rId67" tooltip="Supplier" display="'MMSZ5235B-FDICT-ND" xr:uid="{4E0B8C3E-E37E-4D9C-A0F3-54EF7C005365}"/>
-    <hyperlink ref="F17" r:id="rId68" tooltip="Supplier" display="'F1453CT-ND" xr:uid="{FC4EF832-AD0A-456A-9F0E-D61EE5E10B31}"/>
-    <hyperlink ref="F18" r:id="rId69" tooltip="Supplier" display="'732-4978-1-ND" xr:uid="{DFB914FA-4771-4707-8BCA-ADED281ED2B9}"/>
-    <hyperlink ref="F19" r:id="rId70" tooltip="Supplier" display="'732-4980-1-ND" xr:uid="{3489CECC-DE8B-4FA3-AD86-8FF6846080E9}"/>
-    <hyperlink ref="F20" r:id="rId71" tooltip="Supplier" display="'WM10684-ND" xr:uid="{F40FE0E2-04FD-423F-9667-442B31FDC0B7}"/>
-    <hyperlink ref="F21" r:id="rId72" tooltip="Supplier" display="'WM10862CT-ND" xr:uid="{C23D6CEA-2594-4EEC-A0C9-52898E905217}"/>
-    <hyperlink ref="F22" r:id="rId73" tooltip="Supplier" display="'WM7488-ND" xr:uid="{147F880D-4619-418F-90FF-40452C9A887A}"/>
-    <hyperlink ref="F23" r:id="rId74" tooltip="Supplier" display="'WM10697-ND" xr:uid="{28E1B02F-2ACA-4125-B43A-F6874F162CDF}"/>
-    <hyperlink ref="F24" r:id="rId75" tooltip="Supplier" display="'WM10657-ND" xr:uid="{8791266E-1379-4C58-9EA2-3025D4936789}"/>
-    <hyperlink ref="F25" r:id="rId76" tooltip="Supplier" display="'WM10707-ND" xr:uid="{4872A730-DDE9-4715-9DC9-60D82BCC02A5}"/>
-    <hyperlink ref="F26" r:id="rId77" tooltip="Supplier" display="'NSV1C201MZ4T1GOSCT-ND" xr:uid="{28AD89F8-873C-4BEF-8BAE-8A8240AB63E6}"/>
-    <hyperlink ref="F27" r:id="rId78" tooltip="Supplier" display="'DMP3099L-7DICT-ND" xr:uid="{661AAE38-64DA-4EAA-B624-D7DBA76D2A50}"/>
-    <hyperlink ref="F28" r:id="rId79" tooltip="Supplier" display="'311-100HRCT-ND" xr:uid="{B20C30E2-A5B0-4CE0-A215-3A62A7D99118}"/>
-    <hyperlink ref="F29" r:id="rId80" tooltip="Supplier" display="'541-0.0SBCT-ND" xr:uid="{B966A4A7-DA09-4054-9835-1D305B6E7F68}"/>
-    <hyperlink ref="F30" r:id="rId81" tooltip="Supplier" display="'311-4.70KHRCT-ND" xr:uid="{F7ED8583-5433-4757-8FAB-D43B291E31D7}"/>
-    <hyperlink ref="F31" r:id="rId82" tooltip="Supplier" display="'311-1.40KHRCT-ND" xr:uid="{A0C86976-E8BF-4080-A1E2-658EA68FCC78}"/>
-    <hyperlink ref="F32" r:id="rId83" tooltip="Supplier" display="'311-604HRCT-ND" xr:uid="{D97B5289-620F-420A-8BB0-0C1C77107899}"/>
-    <hyperlink ref="F33" r:id="rId84" tooltip="Supplier" display="'311-100KGRCT-ND" xr:uid="{E30A5747-2E87-40EA-A036-1A6CAB8678E1}"/>
-    <hyperlink ref="F34" r:id="rId85" tooltip="Supplier" display="'P3.3KBYCT-ND" xr:uid="{BCA40196-94F1-4BBC-8025-52FC98C5780F}"/>
-    <hyperlink ref="F35" r:id="rId86" tooltip="Supplier" display="'RPC2512JT33R0CT-ND" xr:uid="{AEEC1122-05A7-4644-8239-4199C90FB251}"/>
-    <hyperlink ref="F36" r:id="rId87" tooltip="Supplier" display="'P62DBCT-ND" xr:uid="{327ABC84-627E-4420-8F3F-0528721D6939}"/>
-    <hyperlink ref="F37" r:id="rId88" tooltip="Supplier" display="'749-1023-1-ND" xr:uid="{F11242F7-5E8C-4AC3-BA5B-B69CC4BE1CD6}"/>
-    <hyperlink ref="F38" r:id="rId89" tooltip="Supplier" display="'490-8601-ND" xr:uid="{8EE49B84-E9D4-4838-9AC7-8292392CF57D}"/>
-    <hyperlink ref="F39" r:id="rId90" tooltip="Supplier" display="'LTC6804IG-1#PBF-ND" xr:uid="{5AE4BCF8-F06F-458B-9659-77063255ED80}"/>
-    <hyperlink ref="F40" r:id="rId91" tooltip="Supplier" display="'296-9226-1-ND" xr:uid="{06049082-D61E-430C-8C86-E0A9C62431A7}"/>
-    <hyperlink ref="F41" r:id="rId92" tooltip="Supplier" display="'296-45323-1-ND" xr:uid="{4A431DEE-6215-4519-821D-7E6A18ECA93C}"/>
-    <hyperlink ref="F42" r:id="rId93" tooltip="Supplier" display="'PT61018AAPEL-SCT-ND" xr:uid="{56562BC9-746A-49AE-8C36-1F4CCDB6DF96}"/>
+    <hyperlink ref="C12" r:id="rId1" tooltip="Component" display="'Murata" xr:uid="{A539BCB9-AC37-44EA-95D3-99D3A616E52E}"/>
+    <hyperlink ref="C13" r:id="rId2" tooltip="Component" display="'Taiyo Yuden" xr:uid="{991DCB86-BE7F-465C-9C7A-4416FEC718FA}"/>
+    <hyperlink ref="C14" r:id="rId3" tooltip="Component" display="'KEMET" xr:uid="{F281B722-59DB-42AB-B63E-37A039B99DF4}"/>
+    <hyperlink ref="C15" r:id="rId4" tooltip="Component" display="'Kyocera AVX" xr:uid="{212191EE-465C-4B63-95F7-253C8BC0823D}"/>
+    <hyperlink ref="C16" r:id="rId5" tooltip="Component" display="'Diodes" xr:uid="{D43C3ADC-1B11-4AB5-AA36-24894614A6CF}"/>
+    <hyperlink ref="C17" r:id="rId6" tooltip="Component" display="'Littelfuse" xr:uid="{0CC162B0-5B02-4499-98E9-F025F94F4997}"/>
+    <hyperlink ref="C18" r:id="rId7" tooltip="Component" display="'Wurth Electronics" xr:uid="{178577D2-B632-4014-AE8F-42B095401ECD}"/>
+    <hyperlink ref="C19" r:id="rId8" tooltip="Component" display="'Wurth Electronics" xr:uid="{128A620F-78F1-44BE-A784-EF8B69F9085B}"/>
+    <hyperlink ref="C20" r:id="rId9" tooltip="Component" display="'Molex" xr:uid="{B34FBE7E-68C7-445B-B5A4-F028DAD8C3EC}"/>
+    <hyperlink ref="C21" r:id="rId10" tooltip="Component" display="'Molex" xr:uid="{8ECB1732-BFBC-42EF-BB63-C00893251463}"/>
+    <hyperlink ref="C22" r:id="rId11" tooltip="Component" display="'Molex" xr:uid="{CC444718-4EFF-43B8-9645-CC4955F306D1}"/>
+    <hyperlink ref="C23" r:id="rId12" tooltip="Component" display="'Molex" xr:uid="{709F251F-F495-470D-8363-1F85C1FFF0BE}"/>
+    <hyperlink ref="C24" r:id="rId13" tooltip="Component" display="'Molex" xr:uid="{C1D70D7D-6847-4DDA-8294-09F0CF76EC5F}"/>
+    <hyperlink ref="C25" r:id="rId14" tooltip="Component" display="'Molex" xr:uid="{0883E227-1920-45E6-A195-CAAD663C39EE}"/>
+    <hyperlink ref="C26" r:id="rId15" tooltip="Component" display="'Molex" xr:uid="{8892887A-364E-40C5-B6BA-82156F6874CD}"/>
+    <hyperlink ref="C27" r:id="rId16" tooltip="Component" display="'ON Semiconductor" xr:uid="{72F3BB34-1B1C-4BCB-98BB-E9E89106A840}"/>
+    <hyperlink ref="C28" r:id="rId17" tooltip="Component" display="'Diodes" xr:uid="{82AF7D91-B9E2-4495-8CE2-74D5A552F0DE}"/>
+    <hyperlink ref="C29" r:id="rId18" tooltip="Component" display="'Yageo" xr:uid="{DB8CD342-5D15-4396-A73F-2B91A2BF9E8E}"/>
+    <hyperlink ref="C30" r:id="rId19" tooltip="Component" display="'Vishay Dale" xr:uid="{5A917341-B48F-4210-A962-25A6D9EB94D5}"/>
+    <hyperlink ref="C31" r:id="rId20" tooltip="Component" display="'Yageo Phycomp" xr:uid="{245875D8-D0D8-48A4-90E3-7785F6DB01DC}"/>
+    <hyperlink ref="C32" r:id="rId21" tooltip="Component" display="'Yageo" xr:uid="{29F864BE-2186-453E-B839-B94736BEF90C}"/>
+    <hyperlink ref="C33" r:id="rId22" tooltip="Component" display="'Yageo" xr:uid="{2641B3D9-41B8-41F9-8BBC-402D04E29097}"/>
+    <hyperlink ref="C34" r:id="rId23" tooltip="Component" display="'Yageo" xr:uid="{4B539E45-B410-48C2-BF7F-9774FDF01A94}"/>
+    <hyperlink ref="C35" r:id="rId24" tooltip="Component" display="'Panasonic" xr:uid="{397189BF-83BF-4807-A7AE-81C5E0B736C2}"/>
+    <hyperlink ref="C36" r:id="rId25" tooltip="Component" display="'Stackpole Electronics" xr:uid="{FE27D9EB-3A01-4E85-9969-099CF0D26D7A}"/>
+    <hyperlink ref="C37" r:id="rId26" tooltip="Component" display="'Panasonic" xr:uid="{190791ED-97BD-4146-B263-0523E75320E2}"/>
+    <hyperlink ref="C38" r:id="rId27" tooltip="Component" display="'Vishay Beyschlag" xr:uid="{8A8946F2-0DFE-4930-8CA7-8721826318A5}"/>
+    <hyperlink ref="C39" r:id="rId28" tooltip="Component" display="'Murata" xr:uid="{B57800D9-C5C4-4F78-A971-9DE6ADA0E9FC}"/>
+    <hyperlink ref="C40" r:id="rId29" tooltip="Component" display="'Analog Devices / Linear Technology" xr:uid="{A5EEB880-02E6-43E7-9EC6-3468F7D09428}"/>
+    <hyperlink ref="C41" r:id="rId30" tooltip="Component" display="'Texas Instruments" xr:uid="{CB6299D8-6793-4D2F-A80A-92358AFF5D15}"/>
+    <hyperlink ref="C42" r:id="rId31" tooltip="Component" display="'Texas Instruments" xr:uid="{75896D2F-102E-4463-A04E-89C4ADAE15F5}"/>
+    <hyperlink ref="C43" r:id="rId32" tooltip="Component" display="'Bourns" xr:uid="{55AB076C-B074-44D5-9071-6B2EEBC54A4F}"/>
+    <hyperlink ref="D12" r:id="rId33" tooltip="Manufacturer" display="'GCM21BR72A104KA37L" xr:uid="{8681C18B-3E24-40F6-9AA2-E5184FD3953E}"/>
+    <hyperlink ref="D13" r:id="rId34" tooltip="Manufacturer" display="'UMK107AB7105KA-T" xr:uid="{677D9DC2-75F5-4C1D-9AA5-5A011DFD3DE7}"/>
+    <hyperlink ref="D14" r:id="rId35" tooltip="Manufacturer" display="'C0603C103J5JAC7867" xr:uid="{A725A531-4EDE-4756-8A8C-C5B307D0B2E1}"/>
+    <hyperlink ref="D15" r:id="rId36" tooltip="Manufacturer" display="'06035C-104KAT2A" xr:uid="{7CA3E41E-9128-4FB9-9EDF-229DC935A28C}"/>
+    <hyperlink ref="D16" r:id="rId37" tooltip="Manufacturer" display="'MMSZ5235B-7-F" xr:uid="{721B0134-4A5D-4328-B5DE-3D6D0C38EDC9}"/>
+    <hyperlink ref="D17" r:id="rId38" tooltip="Manufacturer" display="'0466.375NR" xr:uid="{29B84FED-677E-469D-B956-0B885CAB0970}"/>
+    <hyperlink ref="D18" r:id="rId39" tooltip="Manufacturer" display="'150060RS75000" xr:uid="{DEA6907E-D2BB-4816-BBB0-B662E7904570}"/>
+    <hyperlink ref="D19" r:id="rId40" tooltip="Manufacturer" display="'150060VS75000" xr:uid="{71353F25-FA2D-4FFF-9577-437ABE20C6EB}"/>
+    <hyperlink ref="D20" r:id="rId41" tooltip="Manufacturer" display="'43045-0827" xr:uid="{A5E55097-7B2C-4340-9842-D39A478C8CAD}"/>
+    <hyperlink ref="D21" r:id="rId42" tooltip="Manufacturer" display="'560020-0220" xr:uid="{6F30D106-7657-43BE-91F8-AC8EC8194C8A}"/>
+    <hyperlink ref="D22" r:id="rId43" tooltip="Manufacturer" display="'43045-1027" xr:uid="{328838B3-418B-4CD9-82A5-3CF70167DE77}"/>
+    <hyperlink ref="D23" r:id="rId44" tooltip="Manufacturer" display="'0022284050" xr:uid="{416CE916-D1D0-42ED-84BA-743D652F66C3}"/>
+    <hyperlink ref="D24" r:id="rId45" tooltip="Manufacturer" display="'0430451227" xr:uid="{E82F987E-54A1-4D77-A094-C624FC4CB121}"/>
+    <hyperlink ref="D25" r:id="rId46" tooltip="Manufacturer" display="'43045-0227" xr:uid="{95AB2938-F593-4139-A920-1C2E972CCDEB}"/>
+    <hyperlink ref="D26" r:id="rId47" tooltip="Manufacturer" display="'0430451427" xr:uid="{53CE9709-D24A-40A1-8575-497E32076DDD}"/>
+    <hyperlink ref="D27" r:id="rId48" tooltip="Manufacturer" display="'NSV1C201MZ4T1G" xr:uid="{E8E0EE8E-A3F7-4AB3-B908-F6B04A22390D}"/>
+    <hyperlink ref="D28" r:id="rId49" tooltip="Manufacturer" display="'DMP3099L-7" xr:uid="{851979AF-B02A-4DC1-8D25-32B427258761}"/>
+    <hyperlink ref="D29" r:id="rId50" tooltip="Manufacturer" display="'RC0603FR-07100RL" xr:uid="{0559547B-B0D9-4FF9-8771-FD7EA91CCDB7}"/>
+    <hyperlink ref="D30" r:id="rId51" tooltip="Manufacturer" display="'CRCW06030000Z0EAHP" xr:uid="{81DCD39E-2A04-411C-92FC-9DC9211B2FFD}"/>
+    <hyperlink ref="D31" r:id="rId52" tooltip="Manufacturer" display="'RC0603FR-074K7L" xr:uid="{157BD601-6EC0-4583-9CF8-A1CD01783F39}"/>
+    <hyperlink ref="D32" r:id="rId53" tooltip="Manufacturer" display="'RC0603FR-071K4L" xr:uid="{DEA063DE-8512-48E4-BCB7-2E183CC18E75}"/>
+    <hyperlink ref="D33" r:id="rId54" tooltip="Manufacturer" display="'RC0603FR-07604RL" xr:uid="{64C37259-16E4-4772-91D9-734F80FD30BC}"/>
+    <hyperlink ref="D34" r:id="rId55" tooltip="Manufacturer" display="'RC0603JR-07100KL" xr:uid="{B7149F91-8449-4645-B69C-BCE5D1C98A25}"/>
+    <hyperlink ref="D35" r:id="rId56" tooltip="Manufacturer" display="'ERJPA3F3301V" xr:uid="{2C097292-9292-457E-8421-15091F7FA749}"/>
+    <hyperlink ref="D36" r:id="rId57" tooltip="Manufacturer" display="'RPC2512JT33R0" xr:uid="{06DE3534-8F0D-4918-BA87-349250CE75BA}"/>
+    <hyperlink ref="D37" r:id="rId58" tooltip="Manufacturer" display="'ERA-3AEB620V" xr:uid="{525E86B4-A710-4F69-A165-63E4BA08481D}"/>
+    <hyperlink ref="D38" r:id="rId59" tooltip="Manufacturer" display="'ACASA1002S1002P100" xr:uid="{7B0EC409-3058-49B7-8368-D90DE07954E1}"/>
+    <hyperlink ref="D39" r:id="rId60" tooltip="Manufacturer" display="'NXRT15XH103FA1B030" xr:uid="{08B9BFF4-CDFD-4129-A99E-2969BA43C2D9}"/>
+    <hyperlink ref="D40" r:id="rId61" tooltip="Manufacturer" display="'LTC6804IG-1#PBF" xr:uid="{1F2A4275-8243-490D-A6AE-FA858B5B225C}"/>
+    <hyperlink ref="D41" r:id="rId62" tooltip="Manufacturer" display="'CD74HC4067SM96" xr:uid="{67273A0E-A45D-4ADC-B33D-CC047EAA358C}"/>
+    <hyperlink ref="D42" r:id="rId63" tooltip="Manufacturer" display="'TLV316QDBVRQ1" xr:uid="{AE31C9C2-944D-43E7-BF01-AD6E989DB3E3}"/>
+    <hyperlink ref="D43" r:id="rId64" tooltip="Manufacturer" display="'PT61018AAPEL-S" xr:uid="{D1EE22B8-82A7-49BB-B060-C997CD67FB8B}"/>
+    <hyperlink ref="F12" r:id="rId65" tooltip="Supplier" display="'490-4789-1-ND" xr:uid="{8020F06B-84EC-45AF-BF32-EBF81D98499D}"/>
+    <hyperlink ref="F13" r:id="rId66" tooltip="Supplier" display="'587-3247-1-ND" xr:uid="{20FFFDCD-298B-4250-9666-1DBA9E00CC40}"/>
+    <hyperlink ref="F14" r:id="rId67" tooltip="Supplier" display="'399-13384-1-ND" xr:uid="{D94C7C7E-F685-44FC-8A14-2A48CBF3951D}"/>
+    <hyperlink ref="F15" r:id="rId68" tooltip="Supplier" display="'478-5052-1-ND" xr:uid="{58B33816-57DD-4708-9C42-6A9CC3FCF83A}"/>
+    <hyperlink ref="F16" r:id="rId69" tooltip="Supplier" display="'MMSZ5235B-FDICT-ND" xr:uid="{6204F356-8853-4AF2-8377-9718CD4A8521}"/>
+    <hyperlink ref="F17" r:id="rId70" tooltip="Supplier" display="'F1453CT-ND" xr:uid="{906751B9-F04F-4750-8700-4597B005F583}"/>
+    <hyperlink ref="F18" r:id="rId71" tooltip="Supplier" display="'732-4978-1-ND" xr:uid="{D94D4790-8B5D-4FAF-BBEE-87AAFB79C30F}"/>
+    <hyperlink ref="F19" r:id="rId72" tooltip="Supplier" display="'732-4980-1-ND" xr:uid="{8E7681BB-3541-45F3-AE1B-9CF704782C9A}"/>
+    <hyperlink ref="F20" r:id="rId73" tooltip="Supplier" display="'WM10684-ND" xr:uid="{0403A007-91B5-47DA-AB16-AE50E1DB1707}"/>
+    <hyperlink ref="F21" r:id="rId74" tooltip="Supplier" display="'WM10862CT-ND" xr:uid="{66A059C0-927D-479D-93B8-F1B8951A9A9D}"/>
+    <hyperlink ref="F22" r:id="rId75" tooltip="Supplier" display="'WM7488-ND" xr:uid="{FD04241F-0177-43F5-B074-6702379826D6}"/>
+    <hyperlink ref="F23" r:id="rId76" tooltip="Supplier" display="'WM50014-05-ND" xr:uid="{AC4A7D3F-970A-4FBD-82D4-542A3D4BA331}"/>
+    <hyperlink ref="F24" r:id="rId77" tooltip="Supplier" display="'WM10697-ND" xr:uid="{DBF8CA99-1BEE-482A-91A4-72738B4BBBDA}"/>
+    <hyperlink ref="F25" r:id="rId78" tooltip="Supplier" display="'WM10657-ND" xr:uid="{29ACD268-9F98-4019-9A6D-3C975E14F0CB}"/>
+    <hyperlink ref="F26" r:id="rId79" tooltip="Supplier" display="'WM10707-ND" xr:uid="{7D55A167-77EB-4A44-9027-7331CF4D3F33}"/>
+    <hyperlink ref="F27" r:id="rId80" tooltip="Supplier" display="'NSV1C201MZ4T1GOSCT-ND" xr:uid="{9F6211A1-11F8-4075-B0B8-0F495A4F5CC9}"/>
+    <hyperlink ref="F28" r:id="rId81" tooltip="Supplier" display="'DMP3099L-7DICT-ND" xr:uid="{B8650BB2-0AA4-43E8-B356-DE37FFC5DEBB}"/>
+    <hyperlink ref="F29" r:id="rId82" tooltip="Supplier" display="'311-100HRCT-ND" xr:uid="{7E050433-3F26-46BA-B7C3-4EF753CCC3DC}"/>
+    <hyperlink ref="F30" r:id="rId83" tooltip="Supplier" display="'541-0.0SBCT-ND" xr:uid="{A72BDDA4-B3B1-40B1-A742-1F440F02AAE0}"/>
+    <hyperlink ref="F31" r:id="rId84" tooltip="Supplier" display="'311-4.70KHRCT-ND" xr:uid="{DD26C683-9031-41C2-8619-8833756EC653}"/>
+    <hyperlink ref="F32" r:id="rId85" tooltip="Supplier" display="'311-1.40KHRCT-ND" xr:uid="{8DB5B297-6178-4CDF-AF83-6C2FECA97F23}"/>
+    <hyperlink ref="F33" r:id="rId86" tooltip="Supplier" display="'311-604HRCT-ND" xr:uid="{7598D7E4-3C3F-4FE8-B1EC-E8ACD0B68563}"/>
+    <hyperlink ref="F34" r:id="rId87" tooltip="Supplier" display="'311-100KGRCT-ND" xr:uid="{94D9F5BD-A520-40EF-BD3D-7198758034C1}"/>
+    <hyperlink ref="F35" r:id="rId88" tooltip="Supplier" display="'P3.3KBYCT-ND" xr:uid="{B810D200-A6DD-4E0D-9301-01E17CAD1692}"/>
+    <hyperlink ref="F36" r:id="rId89" tooltip="Supplier" display="'RPC2512JT33R0CT-ND" xr:uid="{9B8DE0B8-43F5-4F7D-A73D-7DDFEA84DA68}"/>
+    <hyperlink ref="F37" r:id="rId90" tooltip="Supplier" display="'P62DBCT-ND" xr:uid="{04347772-C8F9-4CBD-BED0-EF1D74BDBC34}"/>
+    <hyperlink ref="F38" r:id="rId91" tooltip="Supplier" display="'749-1023-1-ND" xr:uid="{6755A851-9829-4142-A1FC-70EC8AE20494}"/>
+    <hyperlink ref="F39" r:id="rId92" tooltip="Supplier" display="'490-8601-ND" xr:uid="{70A29097-79E8-4353-A6A7-09226E74EE42}"/>
+    <hyperlink ref="F40" r:id="rId93" tooltip="Supplier" display="'LTC6804IG-1#PBF-ND" xr:uid="{543D457F-6998-4E7C-9EBA-E42F51322C6C}"/>
+    <hyperlink ref="F41" r:id="rId94" tooltip="Supplier" display="'296-9226-1-ND" xr:uid="{CFB3E3FF-42DA-4D32-88C9-5CDE00C7DA18}"/>
+    <hyperlink ref="F42" r:id="rId95" tooltip="Supplier" display="'296-45323-1-ND" xr:uid="{7A9D3CB1-C828-4989-9362-220EC55B4D9C}"/>
+    <hyperlink ref="F43" r:id="rId96" tooltip="Supplier" display="'PT61018AAPEL-SCT-ND" xr:uid="{BDC3F1BA-12C7-4ADB-88C1-EE1B14F9BB14}"/>
   </hyperlinks>
   <pageMargins left="0.46" right="0.36" top="0.57999999999999996" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId94"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId97"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;BAltium Limited Confidential&amp;B&amp;C&amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId95"/>
+  <drawing r:id="rId98"/>
 </worksheet>
 </file>
 
@@ -2360,7 +2404,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2376,7 +2420,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2392,7 +2436,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2416,7 +2460,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2424,7 +2468,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2448,7 +2492,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2456,7 +2500,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>